<commit_message>
Convert to static site (Oct 2025)
</commit_message>
<xml_diff>
--- a/static/data/Extended-Indexes.xlsx
+++ b/static/data/Extended-Indexes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ437"/>
+  <dimension ref="A1:AQ438"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50678,6 +50678,139 @@
         <v>6.69090909090909</v>
       </c>
     </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>2025-10</t>
+        </is>
+      </c>
+      <c r="B438" t="n">
+        <v>0</v>
+      </c>
+      <c r="C438" t="n">
+        <v>0</v>
+      </c>
+      <c r="D438" t="n">
+        <v>54.54545454545454</v>
+      </c>
+      <c r="E438" t="n">
+        <v>64.70588235294117</v>
+      </c>
+      <c r="F438" t="n">
+        <v>0</v>
+      </c>
+      <c r="G438" t="n">
+        <v>43818.18181818182</v>
+      </c>
+      <c r="H438" t="n">
+        <v>1.055555555555555</v>
+      </c>
+      <c r="I438" t="n">
+        <v>-0.2666666666666666</v>
+      </c>
+      <c r="J438" t="n">
+        <v>2.222222222222222</v>
+      </c>
+      <c r="K438" t="n">
+        <v>-0.2500000000000001</v>
+      </c>
+      <c r="L438" t="n">
+        <v>3.200000000000001</v>
+      </c>
+      <c r="M438" t="n">
+        <v>1.90625</v>
+      </c>
+      <c r="N438" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="O438" t="n">
+        <v>4.080000000000001</v>
+      </c>
+      <c r="P438" t="n">
+        <v>59.59999999999999</v>
+      </c>
+      <c r="Q438" t="n">
+        <v>34.30769230769231</v>
+      </c>
+      <c r="R438" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="S438" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="T438" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="U438" t="n">
+        <v>5.399999999999999</v>
+      </c>
+      <c r="V438" t="n">
+        <v>39.6</v>
+      </c>
+      <c r="W438" t="n">
+        <v>60</v>
+      </c>
+      <c r="X438" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y438" t="n">
+        <v>40</v>
+      </c>
+      <c r="Z438" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA438" t="n">
+        <v>60</v>
+      </c>
+      <c r="AB438" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="AC438" t="n">
+        <v>60</v>
+      </c>
+      <c r="AD438" t="n">
+        <v>68.75</v>
+      </c>
+      <c r="AE438" t="n">
+        <v>13.90909090909091</v>
+      </c>
+      <c r="AF438" t="n">
+        <v>27.55</v>
+      </c>
+      <c r="AG438" t="n">
+        <v>72.72727272727273</v>
+      </c>
+      <c r="AH438" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="AI438" t="n">
+        <v>81.81818181818183</v>
+      </c>
+      <c r="AJ438" t="n">
+        <v>66.66666666666666</v>
+      </c>
+      <c r="AK438" t="n">
+        <v>45.45454545454545</v>
+      </c>
+      <c r="AL438" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="AM438" t="n">
+        <v>3.327272727272728</v>
+      </c>
+      <c r="AN438" t="n">
+        <v>5.227272727272728</v>
+      </c>
+      <c r="AO438" t="n">
+        <v>3.857142857142858</v>
+      </c>
+      <c r="AP438" t="n">
+        <v>4.204545454545454</v>
+      </c>
+      <c r="AQ438" t="n">
+        <v>3.178571428571428</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Convert to static site (Nov 2025)
</commit_message>
<xml_diff>
--- a/static/data/Extended-Indexes.xlsx
+++ b/static/data/Extended-Indexes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ438"/>
+  <dimension ref="A1:AQ439"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50811,6 +50811,139 @@
         <v>3.178571428571428</v>
       </c>
     </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>2025-11</t>
+        </is>
+      </c>
+      <c r="B439" t="n">
+        <v>9.090909090909092</v>
+      </c>
+      <c r="C439" t="n">
+        <v>0</v>
+      </c>
+      <c r="D439" t="n">
+        <v>40</v>
+      </c>
+      <c r="E439" t="n">
+        <v>60.71428571428571</v>
+      </c>
+      <c r="F439" t="n">
+        <v>0</v>
+      </c>
+      <c r="G439" t="n">
+        <v>40166.66666666666</v>
+      </c>
+      <c r="H439" t="n">
+        <v>2.136363636363637</v>
+      </c>
+      <c r="I439" t="n">
+        <v>0.3130434782608695</v>
+      </c>
+      <c r="J439" t="n">
+        <v>3.090909090909091</v>
+      </c>
+      <c r="K439" t="n">
+        <v>0.5065217391304347</v>
+      </c>
+      <c r="L439" t="n">
+        <v>0.4090909090909092</v>
+      </c>
+      <c r="M439" t="n">
+        <v>-0.2260869565217391</v>
+      </c>
+      <c r="N439" t="n">
+        <v>4</v>
+      </c>
+      <c r="O439" t="n">
+        <v>-0.2391304347826086</v>
+      </c>
+      <c r="P439" t="n">
+        <v>59.54545454545455</v>
+      </c>
+      <c r="Q439" t="n">
+        <v>25.93809523809524</v>
+      </c>
+      <c r="R439" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="S439" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="T439" t="n">
+        <v>2</v>
+      </c>
+      <c r="U439" t="n">
+        <v>5</v>
+      </c>
+      <c r="V439" t="n">
+        <v>37.75</v>
+      </c>
+      <c r="W439" t="n">
+        <v>36.36363636363637</v>
+      </c>
+      <c r="X439" t="n">
+        <v>46.42857142857143</v>
+      </c>
+      <c r="Y439" t="n">
+        <v>18.18181818181818</v>
+      </c>
+      <c r="Z439" t="n">
+        <v>18.51851851851852</v>
+      </c>
+      <c r="AA439" t="n">
+        <v>63.63636363636363</v>
+      </c>
+      <c r="AB439" t="n">
+        <v>53.57142857142857</v>
+      </c>
+      <c r="AC439" t="n">
+        <v>81.81818181818183</v>
+      </c>
+      <c r="AD439" t="n">
+        <v>46.42857142857143</v>
+      </c>
+      <c r="AE439" t="n">
+        <v>11.81818181818182</v>
+      </c>
+      <c r="AF439" t="n">
+        <v>28.49999999999999</v>
+      </c>
+      <c r="AG439" t="n">
+        <v>81.81818181818183</v>
+      </c>
+      <c r="AH439" t="n">
+        <v>53.57142857142857</v>
+      </c>
+      <c r="AI439" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ439" t="n">
+        <v>64.28571428571429</v>
+      </c>
+      <c r="AK439" t="n">
+        <v>45.45454545454545</v>
+      </c>
+      <c r="AL439" t="n">
+        <v>40.74074074074074</v>
+      </c>
+      <c r="AM439" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="AN439" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="AO439" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="AP439" t="n">
+        <v>4.527272727272727</v>
+      </c>
+      <c r="AQ439" t="n">
+        <v>3.84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Convert to static site (Dec 2025)
</commit_message>
<xml_diff>
--- a/static/data/Extended-Indexes.xlsx
+++ b/static/data/Extended-Indexes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ439"/>
+  <dimension ref="A1:AQ440"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50944,6 +50944,139 @@
         <v>3.84</v>
       </c>
     </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>2025-12</t>
+        </is>
+      </c>
+      <c r="B440" t="n">
+        <v>0</v>
+      </c>
+      <c r="C440" t="n">
+        <v>9.523809523809524</v>
+      </c>
+      <c r="D440" t="n">
+        <v>25</v>
+      </c>
+      <c r="E440" t="n">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="F440" t="n">
+        <v>0</v>
+      </c>
+      <c r="G440" t="n">
+        <v>40625</v>
+      </c>
+      <c r="H440" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I440" t="n">
+        <v>3.941176470588236</v>
+      </c>
+      <c r="J440" t="n">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="K440" t="n">
+        <v>-1.9375</v>
+      </c>
+      <c r="L440" t="n">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="M440" t="n">
+        <v>-0.8333333333333331</v>
+      </c>
+      <c r="N440" t="n">
+        <v>7.833333333333334</v>
+      </c>
+      <c r="O440" t="n">
+        <v>2.647058823529412</v>
+      </c>
+      <c r="P440" t="n">
+        <v>75.2</v>
+      </c>
+      <c r="Q440" t="n">
+        <v>25.5</v>
+      </c>
+      <c r="R440" t="n">
+        <v>-1</v>
+      </c>
+      <c r="S440" t="n">
+        <v>1</v>
+      </c>
+      <c r="T440" t="n">
+        <v>1</v>
+      </c>
+      <c r="U440" t="n">
+        <v>1</v>
+      </c>
+      <c r="V440" t="n">
+        <v>1</v>
+      </c>
+      <c r="W440" t="n">
+        <v>71.42857142857143</v>
+      </c>
+      <c r="X440" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y440" t="n">
+        <v>28.57142857142857</v>
+      </c>
+      <c r="Z440" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA440" t="n">
+        <v>50</v>
+      </c>
+      <c r="AB440" t="n">
+        <v>85</v>
+      </c>
+      <c r="AC440" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="AD440" t="n">
+        <v>52.63157894736842</v>
+      </c>
+      <c r="AE440" t="n">
+        <v>17.375</v>
+      </c>
+      <c r="AF440" t="n">
+        <v>18.94736842105263</v>
+      </c>
+      <c r="AG440" t="n">
+        <v>57.14285714285714</v>
+      </c>
+      <c r="AH440" t="n">
+        <v>52.38095238095239</v>
+      </c>
+      <c r="AI440" t="n">
+        <v>100</v>
+      </c>
+      <c r="AJ440" t="n">
+        <v>61.90476190476191</v>
+      </c>
+      <c r="AK440" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="AL440" t="n">
+        <v>35</v>
+      </c>
+      <c r="AM440" t="n">
+        <v>4.300000000000001</v>
+      </c>
+      <c r="AN440" t="n">
+        <v>8.071428571428571</v>
+      </c>
+      <c r="AO440" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="AP440" t="n">
+        <v>7.714285714285715</v>
+      </c>
+      <c r="AQ440" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Convert to static site (Jan 2026)
</commit_message>
<xml_diff>
--- a/static/data/Extended-Indexes.xlsx
+++ b/static/data/Extended-Indexes.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ440"/>
+  <dimension ref="A1:AQ441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -50954,13 +50954,13 @@
         <v>0</v>
       </c>
       <c r="C440" t="n">
-        <v>9.523809523809524</v>
+        <v>8</v>
       </c>
       <c r="D440" t="n">
         <v>25</v>
       </c>
       <c r="E440" t="n">
-        <v>71.42857142857143</v>
+        <v>72</v>
       </c>
       <c r="F440" t="n">
         <v>0</v>
@@ -50972,31 +50972,31 @@
         <v>0.25</v>
       </c>
       <c r="I440" t="n">
-        <v>3.941176470588236</v>
+        <v>3.45</v>
       </c>
       <c r="J440" t="n">
         <v>1.666666666666667</v>
       </c>
       <c r="K440" t="n">
-        <v>-1.9375</v>
+        <v>-1.947368421052632</v>
       </c>
       <c r="L440" t="n">
         <v>3.333333333333333</v>
       </c>
       <c r="M440" t="n">
-        <v>-0.8333333333333331</v>
+        <v>-0.7619047619047619</v>
       </c>
       <c r="N440" t="n">
         <v>7.833333333333334</v>
       </c>
       <c r="O440" t="n">
-        <v>2.647058823529412</v>
+        <v>2.326190476190476</v>
       </c>
       <c r="P440" t="n">
         <v>75.2</v>
       </c>
       <c r="Q440" t="n">
-        <v>25.5</v>
+        <v>29.59523809523809</v>
       </c>
       <c r="R440" t="n">
         <v>-1</v>
@@ -51017,49 +51017,49 @@
         <v>71.42857142857143</v>
       </c>
       <c r="X440" t="n">
-        <v>50</v>
+        <v>45.83333333333333</v>
       </c>
       <c r="Y440" t="n">
         <v>28.57142857142857</v>
       </c>
       <c r="Z440" t="n">
-        <v>30</v>
+        <v>37.5</v>
       </c>
       <c r="AA440" t="n">
         <v>50</v>
       </c>
       <c r="AB440" t="n">
-        <v>85</v>
+        <v>79.16666666666666</v>
       </c>
       <c r="AC440" t="n">
         <v>62.5</v>
       </c>
       <c r="AD440" t="n">
-        <v>52.63157894736842</v>
+        <v>52.17391304347826</v>
       </c>
       <c r="AE440" t="n">
         <v>17.375</v>
       </c>
       <c r="AF440" t="n">
-        <v>18.94736842105263</v>
+        <v>20.21739130434783</v>
       </c>
       <c r="AG440" t="n">
         <v>57.14285714285714</v>
       </c>
       <c r="AH440" t="n">
-        <v>52.38095238095239</v>
+        <v>56.00000000000001</v>
       </c>
       <c r="AI440" t="n">
         <v>100</v>
       </c>
       <c r="AJ440" t="n">
-        <v>61.90476190476191</v>
+        <v>64</v>
       </c>
       <c r="AK440" t="n">
         <v>62.5</v>
       </c>
       <c r="AL440" t="n">
-        <v>35</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="AM440" t="n">
         <v>4.300000000000001</v>
@@ -51075,6 +51075,139 @@
       </c>
       <c r="AQ440" t="n">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>2026-01</t>
+        </is>
+      </c>
+      <c r="B441" t="n">
+        <v>16.66666666666666</v>
+      </c>
+      <c r="C441" t="n">
+        <v>0</v>
+      </c>
+      <c r="D441" t="n">
+        <v>58.33333333333334</v>
+      </c>
+      <c r="E441" t="n">
+        <v>76.92307692307693</v>
+      </c>
+      <c r="F441" t="n">
+        <v>16.66666666666666</v>
+      </c>
+      <c r="G441" t="n">
+        <v>40916.41666666666</v>
+      </c>
+      <c r="H441" t="n">
+        <v>-0.4444444444444444</v>
+      </c>
+      <c r="I441" t="n">
+        <v>-0.3750000000000001</v>
+      </c>
+      <c r="J441" t="n">
+        <v>0</v>
+      </c>
+      <c r="K441" t="n">
+        <v>-0.8333333333333334</v>
+      </c>
+      <c r="L441" t="n">
+        <v>3.888888888888889</v>
+      </c>
+      <c r="M441" t="n">
+        <v>-0.3749999999999998</v>
+      </c>
+      <c r="N441" t="n">
+        <v>6.909090909090909</v>
+      </c>
+      <c r="O441" t="n">
+        <v>3.772727272727272</v>
+      </c>
+      <c r="P441" t="n">
+        <v>43.22727272727272</v>
+      </c>
+      <c r="Q441" t="n">
+        <v>56.89999999999999</v>
+      </c>
+      <c r="R441" t="n">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="S441" t="n">
+        <v>2.333333333333333</v>
+      </c>
+      <c r="T441" t="n">
+        <v>4.333333333333334</v>
+      </c>
+      <c r="U441" t="n">
+        <v>7.249999999999999</v>
+      </c>
+      <c r="V441" t="n">
+        <v>36.25</v>
+      </c>
+      <c r="W441" t="n">
+        <v>33.33333333333333</v>
+      </c>
+      <c r="X441" t="n">
+        <v>69.23076923076923</v>
+      </c>
+      <c r="Y441" t="n">
+        <v>8.333333333333332</v>
+      </c>
+      <c r="Z441" t="n">
+        <v>41.66666666666667</v>
+      </c>
+      <c r="AA441" t="n">
+        <v>75</v>
+      </c>
+      <c r="AB441" t="n">
+        <v>76.92307692307693</v>
+      </c>
+      <c r="AC441" t="n">
+        <v>58.33333333333334</v>
+      </c>
+      <c r="AD441" t="n">
+        <v>46.15384615384615</v>
+      </c>
+      <c r="AE441" t="n">
+        <v>23.75</v>
+      </c>
+      <c r="AF441" t="n">
+        <v>24.03846153846154</v>
+      </c>
+      <c r="AG441" t="n">
+        <v>41.66666666666667</v>
+      </c>
+      <c r="AH441" t="n">
+        <v>76.92307692307693</v>
+      </c>
+      <c r="AI441" t="n">
+        <v>66.66666666666666</v>
+      </c>
+      <c r="AJ441" t="n">
+        <v>84.61538461538461</v>
+      </c>
+      <c r="AK441" t="n">
+        <v>58.33333333333334</v>
+      </c>
+      <c r="AL441" t="n">
+        <v>30.76923076923077</v>
+      </c>
+      <c r="AM441" t="n">
+        <v>3.229166666666667</v>
+      </c>
+      <c r="AN441" t="n">
+        <v>8.375</v>
+      </c>
+      <c r="AO441" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="AP441" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="AQ441" t="n">
+        <v>17.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>